<commit_message>
Working on killing enemy
left to do: kill all enemies in area
</commit_message>
<xml_diff>
--- a/Assets/ToDo.xlsx
+++ b/Assets/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\Main\Studia\Silniki\LightPlatformer\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F7C656-B680-4B72-A4B9-F40B94F92B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015A58ED-C0B5-468F-A52D-EDFA49A7F084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t>Status</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Add script for auto shadow cast 2d for tilemap (ask Dawid for script)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>wysłać maila jak usuwać przeciwników od najbliższego do najdalszego (sortowanie listy po odległości</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,9 +551,10 @@
     <col min="3" max="3" width="46.44140625" customWidth="1"/>
     <col min="4" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -555,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>19</v>
@@ -566,8 +573,11 @@
       <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -586,8 +596,11 @@
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -606,8 +619,9 @@
       <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -626,8 +640,9 @@
       <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -646,8 +661,9 @@
       <c r="F5" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -666,8 +682,9 @@
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -686,8 +703,9 @@
       <c r="F7" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -706,8 +724,9 @@
       <c r="F8" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -726,8 +745,9 @@
       <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -746,8 +766,9 @@
       <c r="F10" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -755,7 +776,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>

</xml_diff>